<commit_message>
updated and added points 3,4.1
</commit_message>
<xml_diff>
--- a/MarketData_4.xlsx
+++ b/MarketData_4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\OneDrive\Desktop\Samuele\Università\IV Anno\MATHEMATICAL FINANCE II\LAB\Project_LV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF4F39E-A029-4991-9642-24F25E81869A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3FE9FA1-05FB-4729-9B96-1F4492F94B4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="E CORP" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -113,7 +113,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="8">
+  <numFmts count="9">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$-409]dd\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
@@ -122,6 +122,7 @@
     <numFmt numFmtId="168" formatCode="0.00000"/>
     <numFmt numFmtId="169" formatCode="0.000000"/>
     <numFmt numFmtId="170" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="174" formatCode="0.0000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -542,7 +543,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Migliaia" xfId="2" builtinId="3"/>
@@ -7542,8 +7543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7800,29 +7801,29 @@
         <v>0.28799999999999998</v>
       </c>
       <c r="J13" s="56"/>
-      <c r="K13" s="67" cm="1">
+      <c r="K13" cm="1">
         <f t="array" ref="K13:R19">B13:I19</f>
         <v>0.16520000000000001</v>
       </c>
-      <c r="L13" s="67">
+      <c r="L13">
         <v>0.21809999999999999</v>
       </c>
-      <c r="M13" s="67">
+      <c r="M13">
         <v>0.25490000000000002</v>
       </c>
-      <c r="N13" s="67">
+      <c r="N13">
         <v>0.27439999999999998</v>
       </c>
-      <c r="O13" s="67">
+      <c r="O13">
         <v>0.27489999999999998</v>
       </c>
-      <c r="P13" s="67">
+      <c r="P13">
         <v>0.28389999999999999</v>
       </c>
-      <c r="Q13" s="67">
+      <c r="Q13">
         <v>0.28139999999999998</v>
       </c>
-      <c r="R13" s="67">
+      <c r="R13">
         <v>0.28799999999999998</v>
       </c>
     </row>
@@ -7853,28 +7854,28 @@
         <v>0.20730000000000001</v>
       </c>
       <c r="J14" s="56"/>
-      <c r="K14" s="67">
+      <c r="K14">
         <v>0.1074</v>
       </c>
-      <c r="L14" s="67">
+      <c r="L14">
         <v>0.15090000000000001</v>
       </c>
-      <c r="M14" s="67">
+      <c r="M14">
         <v>0.17699999999999999</v>
       </c>
-      <c r="N14" s="67">
+      <c r="N14">
         <v>0.18890000000000001</v>
       </c>
-      <c r="O14" s="67">
+      <c r="O14">
         <v>0.19239999999999999</v>
       </c>
-      <c r="P14" s="67">
+      <c r="P14">
         <v>0.20280000000000001</v>
       </c>
-      <c r="Q14" s="67">
+      <c r="Q14">
         <v>0.20430000000000001</v>
       </c>
-      <c r="R14" s="67">
+      <c r="R14">
         <v>0.20730000000000001</v>
       </c>
     </row>
@@ -7905,28 +7906,28 @@
         <v>0.18770000000000001</v>
       </c>
       <c r="J15" s="56"/>
-      <c r="K15" s="67">
+      <c r="K15">
         <v>9.35E-2</v>
       </c>
-      <c r="L15" s="67">
+      <c r="L15">
         <v>0.1351</v>
       </c>
-      <c r="M15" s="67">
+      <c r="M15">
         <v>0.15290000000000001</v>
       </c>
-      <c r="N15" s="67">
+      <c r="N15">
         <v>0.16339999999999999</v>
       </c>
-      <c r="O15" s="67">
+      <c r="O15">
         <v>0.1716</v>
       </c>
-      <c r="P15" s="67">
+      <c r="P15">
         <v>0.17879999999999999</v>
       </c>
-      <c r="Q15" s="67">
+      <c r="Q15">
         <v>0.1822</v>
       </c>
-      <c r="R15" s="67">
+      <c r="R15">
         <v>0.18770000000000001</v>
       </c>
     </row>
@@ -7957,28 +7958,28 @@
         <v>0.17730000000000001</v>
       </c>
       <c r="J16" s="56"/>
-      <c r="K16" s="67">
+      <c r="K16">
         <v>8.3199999999999996E-2</v>
       </c>
-      <c r="L16" s="67">
+      <c r="L16">
         <v>0.12740000000000001</v>
       </c>
-      <c r="M16" s="67">
+      <c r="M16">
         <v>0.14119999999999999</v>
       </c>
-      <c r="N16" s="67">
+      <c r="N16">
         <v>0.14879999999999999</v>
       </c>
-      <c r="O16" s="67">
+      <c r="O16">
         <v>0.15970000000000001</v>
       </c>
-      <c r="P16" s="67">
+      <c r="P16">
         <v>0.1691</v>
       </c>
-      <c r="Q16" s="67">
+      <c r="Q16">
         <v>0.17230000000000001</v>
       </c>
-      <c r="R16" s="67">
+      <c r="R16">
         <v>0.17730000000000001</v>
       </c>
     </row>
@@ -8009,28 +8010,28 @@
         <v>0.16819999999999999</v>
       </c>
       <c r="J17" s="56"/>
-      <c r="K17" s="67">
+      <c r="K17">
         <v>7.7700000000000005E-2</v>
       </c>
-      <c r="L17" s="67">
+      <c r="L17">
         <v>0.1137</v>
       </c>
-      <c r="M17" s="67">
+      <c r="M17">
         <v>0.13569999999999999</v>
       </c>
-      <c r="N17" s="67">
+      <c r="N17">
         <v>0.1401</v>
       </c>
-      <c r="O17" s="67">
+      <c r="O17">
         <v>0.14860000000000001</v>
       </c>
-      <c r="P17" s="67">
+      <c r="P17">
         <v>0.1573</v>
       </c>
-      <c r="Q17" s="67">
+      <c r="Q17">
         <v>0.16339999999999999</v>
       </c>
-      <c r="R17" s="67">
+      <c r="R17">
         <v>0.16819999999999999</v>
       </c>
     </row>
@@ -8061,28 +8062,28 @@
         <v>0.15870000000000001</v>
       </c>
       <c r="J18" s="56"/>
-      <c r="K18" s="67">
+      <c r="K18">
         <v>7.6799999999999993E-2</v>
       </c>
-      <c r="L18" s="67">
+      <c r="L18">
         <v>0.10780000000000001</v>
       </c>
-      <c r="M18" s="67">
+      <c r="M18">
         <v>0.12230000000000001</v>
       </c>
-      <c r="N18" s="67">
+      <c r="N18">
         <v>0.1295</v>
       </c>
-      <c r="O18" s="67">
+      <c r="O18">
         <v>0.13639999999999999</v>
       </c>
-      <c r="P18" s="67">
+      <c r="P18">
         <v>0.14580000000000001</v>
       </c>
-      <c r="Q18" s="67">
+      <c r="Q18">
         <v>0.1527</v>
       </c>
-      <c r="R18" s="67">
+      <c r="R18">
         <v>0.15870000000000001</v>
       </c>
     </row>
@@ -8113,28 +8114,28 @@
         <v>0.14749999999999999</v>
       </c>
       <c r="J19" s="56"/>
-      <c r="K19" s="67">
+      <c r="K19">
         <v>7.9299999999999995E-2</v>
       </c>
-      <c r="L19" s="67">
+      <c r="L19">
         <v>9.8400000000000001E-2</v>
       </c>
-      <c r="M19" s="67">
+      <c r="M19">
         <v>0.1085</v>
       </c>
-      <c r="N19" s="67">
+      <c r="N19">
         <v>0.1144</v>
       </c>
-      <c r="O19" s="67">
+      <c r="O19">
         <v>0.11990000000000001</v>
       </c>
-      <c r="P19" s="67">
+      <c r="P19">
         <v>0.13089999999999999</v>
       </c>
-      <c r="Q19" s="67">
+      <c r="Q19">
         <v>0.13750000000000001</v>
       </c>
-      <c r="R19" s="67">
+      <c r="R19">
         <v>0.14749999999999999</v>
       </c>
     </row>
@@ -8395,10 +8396,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:J18"/>
+  <dimension ref="A2:P18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8408,7 +8409,7 @@
     <col min="3" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>6</v>
       </c>
@@ -8422,7 +8423,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="58"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -8436,7 +8437,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="59"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -8450,7 +8451,7 @@
       <c r="G4" s="12"/>
       <c r="H4" s="14"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>3</v>
       </c>
@@ -8478,7 +8479,7 @@
       <c r="I5" s="57"/>
       <c r="J5" s="57"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -8511,7 +8512,7 @@
         <v>1.010958904109589</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -8537,7 +8538,7 @@
         <v>0.98044500000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -8570,7 +8571,7 @@
         <v>1.0026841394444914</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="33" t="s">
         <v>2</v>
       </c>
@@ -8596,7 +8597,7 @@
         <v>1.207686</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -8608,7 +8609,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="58"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>11</v>
       </c>
@@ -8643,7 +8644,7 @@
       <c r="I13" s="57"/>
       <c r="J13" s="57"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="44">
         <v>10</v>
       </c>
@@ -8669,9 +8670,30 @@
         <v>7.9380399557279505E-2</v>
       </c>
       <c r="I14" s="56"/>
-      <c r="J14" s="56"/>
+      <c r="J14" s="67" cm="1">
+        <f t="array" ref="J14:P18">B14:H18</f>
+        <v>7.28420967861481E-2</v>
+      </c>
+      <c r="K14" s="67">
+        <v>6.4896246225656304E-2</v>
+      </c>
+      <c r="L14" s="67">
+        <v>6.5435828882835903E-2</v>
+      </c>
+      <c r="M14" s="67">
+        <v>7.6120381620218502E-2</v>
+      </c>
+      <c r="N14" s="67">
+        <v>7.5761989527394893E-2</v>
+      </c>
+      <c r="O14" s="67">
+        <v>7.7481028258743603E-2</v>
+      </c>
+      <c r="P14" s="67">
+        <v>7.9380399557279505E-2</v>
+      </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="45">
         <v>25</v>
       </c>
@@ -8697,9 +8719,29 @@
         <v>7.5250680231498598E-2</v>
       </c>
       <c r="I15" s="56"/>
-      <c r="J15" s="56"/>
+      <c r="J15" s="67">
+        <v>6.7591160524062097E-2</v>
+      </c>
+      <c r="K15" s="67">
+        <v>5.7149221059707302E-2</v>
+      </c>
+      <c r="L15" s="67">
+        <v>6.1758192773473698E-2</v>
+      </c>
+      <c r="M15" s="67">
+        <v>7.2631788121527596E-2</v>
+      </c>
+      <c r="N15" s="67">
+        <v>7.2015666212843193E-2</v>
+      </c>
+      <c r="O15" s="67">
+        <v>7.4099271286331606E-2</v>
+      </c>
+      <c r="P15" s="67">
+        <v>7.5250680231498598E-2</v>
+      </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="45">
         <v>50</v>
       </c>
@@ -8725,9 +8767,29 @@
         <v>7.4308084832583998E-2</v>
       </c>
       <c r="I16" s="56"/>
-      <c r="J16" s="56"/>
+      <c r="J16" s="67">
+        <v>6.4659056853264604E-2</v>
+      </c>
+      <c r="K16" s="67">
+        <v>5.73787094750835E-2</v>
+      </c>
+      <c r="L16" s="67">
+        <v>6.0844357096339598E-2</v>
+      </c>
+      <c r="M16" s="67">
+        <v>7.0767219030693496E-2</v>
+      </c>
+      <c r="N16" s="67">
+        <v>7.0898695814719997E-2</v>
+      </c>
+      <c r="O16" s="67">
+        <v>7.3041122671170605E-2</v>
+      </c>
+      <c r="P16" s="67">
+        <v>7.4308084832583998E-2</v>
+      </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="45">
         <v>75</v>
       </c>
@@ -8753,9 +8815,29 @@
         <v>7.7449311461341902E-2</v>
       </c>
       <c r="I17" s="56"/>
-      <c r="J17" s="56"/>
+      <c r="J17" s="67">
+        <v>6.1035414327573798E-2</v>
+      </c>
+      <c r="K17" s="67">
+        <v>5.94410875980734E-2</v>
+      </c>
+      <c r="L17" s="67">
+        <v>6.3119248034155695E-2</v>
+      </c>
+      <c r="M17" s="67">
+        <v>7.2027860126685495E-2</v>
+      </c>
+      <c r="N17" s="67">
+        <v>7.3410459718974697E-2</v>
+      </c>
+      <c r="O17" s="67">
+        <v>7.5847761168901698E-2</v>
+      </c>
+      <c r="P17" s="67">
+        <v>7.7449311461341902E-2</v>
+      </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="46">
         <v>90</v>
       </c>
@@ -8781,22 +8863,43 @@
         <v>8.3531741245736799E-2</v>
       </c>
       <c r="I18" s="56"/>
-      <c r="J18" s="56"/>
+      <c r="J18" s="67">
+        <v>6.7613431940314897E-2</v>
+      </c>
+      <c r="K18" s="67">
+        <v>6.16917518485589E-2</v>
+      </c>
+      <c r="L18" s="67">
+        <v>6.6479201525611306E-2</v>
+      </c>
+      <c r="M18" s="67">
+        <v>7.5431733516237706E-2</v>
+      </c>
+      <c r="N18" s="67">
+        <v>7.8536030618170202E-2</v>
+      </c>
+      <c r="O18" s="67">
+        <v>8.0742341083799504E-2</v>
+      </c>
+      <c r="P18" s="67">
+        <v>8.3531741245736799E-2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B3:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:C26"/>
+  <dimension ref="A2:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8805,7 +8908,7 @@
     <col min="2" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>6</v>
       </c>
@@ -8814,7 +8917,7 @@
       </c>
       <c r="C2" s="47"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -8823,7 +8926,7 @@
       </c>
       <c r="C3" s="66"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -8832,7 +8935,7 @@
       </c>
       <c r="C4" s="14"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>3</v>
       </c>
@@ -8843,7 +8946,7 @@
         <v>43827</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -8856,7 +8959,7 @@
         <v>3.287671232876712E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>8</v>
       </c>
@@ -8867,7 +8970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="33" t="s">
         <v>2</v>
       </c>
@@ -8878,14 +8981,14 @@
         <v>4.5070829999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="47"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>3</v>
       </c>
@@ -8898,7 +9001,7 @@
         <v>43827</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="27"/>
       <c r="B13" s="19">
         <v>0.19025</v>
@@ -8906,8 +9009,15 @@
       <c r="C13" s="16">
         <v>0.12025</v>
       </c>
+      <c r="E13" s="67" cm="1">
+        <f t="array" ref="E13:F17">B13:C17</f>
+        <v>0.19025</v>
+      </c>
+      <c r="F13" s="67">
+        <v>0.12025</v>
+      </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="28"/>
       <c r="B14" s="20">
         <v>0.19750000000000001</v>
@@ -8915,8 +9025,14 @@
       <c r="C14" s="17">
         <v>0.1275</v>
       </c>
+      <c r="E14" s="67">
+        <v>0.19750000000000001</v>
+      </c>
+      <c r="F14" s="67">
+        <v>0.1275</v>
+      </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="28"/>
       <c r="B15" s="20">
         <v>0.20499999999999999</v>
@@ -8924,8 +9040,14 @@
       <c r="C15" s="17">
         <v>0.13500000000000001</v>
       </c>
+      <c r="E15" s="67">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="F15" s="67">
+        <v>0.13500000000000001</v>
+      </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="28"/>
       <c r="B16" s="20">
         <v>0.41749999999999998</v>
@@ -8933,8 +9055,14 @@
       <c r="C16" s="17">
         <v>0.14749999999999999</v>
       </c>
+      <c r="E16" s="67">
+        <v>0.41749999999999998</v>
+      </c>
+      <c r="F16" s="67">
+        <v>0.14749999999999999</v>
+      </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="29"/>
       <c r="B17" s="32">
         <v>0.23225000000000001</v>
@@ -8942,15 +9070,21 @@
       <c r="C17" s="31">
         <v>0.16225000000000001</v>
       </c>
+      <c r="E17" s="67">
+        <v>0.23225000000000001</v>
+      </c>
+      <c r="F17" s="67">
+        <v>0.16225000000000001</v>
+      </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="47"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
         <v>3</v>
       </c>
@@ -8963,7 +9097,7 @@
         <v>43827</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="27"/>
       <c r="B22" s="50">
         <v>4.4106011347600003</v>
@@ -8972,7 +9106,7 @@
         <v>4.4106011347600003</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="28"/>
       <c r="B23" s="52">
         <v>4.4547925892320004</v>
@@ -8981,7 +9115,7 @@
         <v>4.4547925892320004</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="28"/>
       <c r="B24" s="52">
         <v>4.5080919651440006</v>
@@ -8990,7 +9124,7 @@
         <v>4.5080919651440006</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="28"/>
       <c r="B25" s="52">
         <v>4.5692953936720002</v>
@@ -8999,7 +9133,7 @@
         <v>4.5692953936720002</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="29"/>
       <c r="B26" s="54">
         <v>4.6326675896319998</v>

</xml_diff>